<commit_message>
falta so o estatistico
</commit_message>
<xml_diff>
--- a/SPES01-2024-09_Potencial.xlsx
+++ b/SPES01-2024-09_Potencial.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="14">
   <si>
     <t>Nome</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>PR</t>
-  </si>
-  <si>
-    <t>['Hora', 'Avg']</t>
   </si>
 </sst>
 </file>
@@ -416,13 +413,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AX26"/>
+  <dimension ref="A1:AY25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:50">
+    <row r="1" spans="1:51">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,14 +548,17 @@
         <v>4</v>
       </c>
       <c r="AV1" s="1"/>
-      <c r="AW1" s="1">
-        <v>0</v>
-      </c>
-      <c r="AX1" s="1">
+      <c r="AW1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="AY1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:50">
+    <row r="2" spans="1:51">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -682,11 +682,14 @@
       <c r="AW2" t="s">
         <v>13</v>
       </c>
-      <c r="AX2" t="s">
-        <v>14</v>
+      <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:50">
+    <row r="3" spans="1:51">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -807,14 +810,17 @@
       <c r="AU3">
         <v>946.095</v>
       </c>
-      <c r="AW3">
-        <v>0</v>
+      <c r="AW3" t="s">
+        <v>13</v>
       </c>
       <c r="AX3">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AY3">
+        <v>0.008466666666666667</v>
       </c>
     </row>
-    <row r="4" spans="1:50">
+    <row r="4" spans="1:51">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -935,14 +941,17 @@
       <c r="AU4">
         <v>945.866111111111</v>
       </c>
-      <c r="AW4">
-        <v>1</v>
+      <c r="AW4" t="s">
+        <v>13</v>
       </c>
       <c r="AX4">
-        <v>0.008466666666666667</v>
+        <v>2</v>
+      </c>
+      <c r="AY4">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:50">
+    <row r="5" spans="1:51">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1063,14 +1072,17 @@
       <c r="AU5">
         <v>945.7149999999999</v>
       </c>
-      <c r="AW5">
-        <v>2</v>
+      <c r="AW5" t="s">
+        <v>13</v>
       </c>
       <c r="AX5">
+        <v>3</v>
+      </c>
+      <c r="AY5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:50">
+    <row r="6" spans="1:51">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1191,14 +1203,17 @@
       <c r="AU6">
         <v>945.5915555555554</v>
       </c>
-      <c r="AW6">
-        <v>3</v>
+      <c r="AW6" t="s">
+        <v>13</v>
       </c>
       <c r="AX6">
+        <v>4</v>
+      </c>
+      <c r="AY6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:50">
+    <row r="7" spans="1:51">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1319,14 +1334,17 @@
       <c r="AU7">
         <v>946.2972222222221</v>
       </c>
-      <c r="AW7">
-        <v>4</v>
+      <c r="AW7" t="s">
+        <v>13</v>
       </c>
       <c r="AX7">
+        <v>5</v>
+      </c>
+      <c r="AY7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:50">
+    <row r="8" spans="1:51">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1447,14 +1465,17 @@
       <c r="AU8">
         <v>946.6813079096044</v>
       </c>
-      <c r="AW8">
-        <v>5</v>
+      <c r="AW8" t="s">
+        <v>13</v>
       </c>
       <c r="AX8">
+        <v>6</v>
+      </c>
+      <c r="AY8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:50">
+    <row r="9" spans="1:51">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1575,14 +1596,17 @@
       <c r="AU9">
         <v>946.5977667271628</v>
       </c>
-      <c r="AW9">
-        <v>6</v>
+      <c r="AW9" t="s">
+        <v>13</v>
       </c>
       <c r="AX9">
+        <v>7</v>
+      </c>
+      <c r="AY9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:50">
+    <row r="10" spans="1:51">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1703,14 +1727,17 @@
       <c r="AU10">
         <v>948.2027777777779</v>
       </c>
-      <c r="AW10">
-        <v>7</v>
+      <c r="AW10" t="s">
+        <v>13</v>
       </c>
       <c r="AX10">
+        <v>8</v>
+      </c>
+      <c r="AY10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:50">
+    <row r="11" spans="1:51">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1831,14 +1858,17 @@
       <c r="AU11">
         <v>948.3583333333333</v>
       </c>
-      <c r="AW11">
-        <v>8</v>
+      <c r="AW11" t="s">
+        <v>13</v>
       </c>
       <c r="AX11">
+        <v>9</v>
+      </c>
+      <c r="AY11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:50">
+    <row r="12" spans="1:51">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1959,14 +1989,17 @@
       <c r="AU12">
         <v>947.7447363465161</v>
       </c>
-      <c r="AW12">
-        <v>9</v>
+      <c r="AW12" t="s">
+        <v>13</v>
       </c>
       <c r="AX12">
+        <v>10</v>
+      </c>
+      <c r="AY12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:50">
+    <row r="13" spans="1:51">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -2087,14 +2120,17 @@
       <c r="AU13">
         <v>947.0505838041431</v>
       </c>
-      <c r="AW13">
-        <v>10</v>
+      <c r="AW13" t="s">
+        <v>13</v>
       </c>
       <c r="AX13">
+        <v>11</v>
+      </c>
+      <c r="AY13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:50">
+    <row r="14" spans="1:51">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -2215,14 +2251,17 @@
       <c r="AU14">
         <v>946.3377777777775</v>
       </c>
-      <c r="AW14">
-        <v>11</v>
+      <c r="AW14" t="s">
+        <v>13</v>
       </c>
       <c r="AX14">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="AY14">
+        <v>0.008466666666666667</v>
       </c>
     </row>
-    <row r="15" spans="1:50">
+    <row r="15" spans="1:51">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -2343,14 +2382,17 @@
       <c r="AU15">
         <v>945.2722222222221</v>
       </c>
-      <c r="AW15">
-        <v>12</v>
+      <c r="AW15" t="s">
+        <v>13</v>
       </c>
       <c r="AX15">
-        <v>0.008466666666666667</v>
+        <v>13</v>
+      </c>
+      <c r="AY15">
+        <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:50">
+    <row r="16" spans="1:51">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -2471,14 +2513,17 @@
       <c r="AU16">
         <v>944.1029444444445</v>
       </c>
-      <c r="AW16">
+      <c r="AW16" t="s">
         <v>13</v>
       </c>
       <c r="AX16">
+        <v>14</v>
+      </c>
+      <c r="AY16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:50">
+    <row r="17" spans="1:51">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -2599,14 +2644,17 @@
       <c r="AU17">
         <v>943.6388333333331</v>
       </c>
-      <c r="AW17">
-        <v>14</v>
+      <c r="AW17" t="s">
+        <v>13</v>
       </c>
       <c r="AX17">
+        <v>15</v>
+      </c>
+      <c r="AY17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:50">
+    <row r="18" spans="1:51">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -2727,14 +2775,17 @@
       <c r="AU18">
         <v>943.6366666666668</v>
       </c>
-      <c r="AW18">
-        <v>15</v>
+      <c r="AW18" t="s">
+        <v>13</v>
       </c>
       <c r="AX18">
+        <v>16</v>
+      </c>
+      <c r="AY18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:50">
+    <row r="19" spans="1:51">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -2855,14 +2906,17 @@
       <c r="AU19">
         <v>943.9333333333333</v>
       </c>
-      <c r="AW19">
-        <v>16</v>
+      <c r="AW19" t="s">
+        <v>13</v>
       </c>
       <c r="AX19">
+        <v>17</v>
+      </c>
+      <c r="AY19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:50">
+    <row r="20" spans="1:51">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -2983,14 +3037,17 @@
       <c r="AU20">
         <v>944.4527777777778</v>
       </c>
-      <c r="AW20">
-        <v>17</v>
+      <c r="AW20" t="s">
+        <v>13</v>
       </c>
       <c r="AX20">
+        <v>18</v>
+      </c>
+      <c r="AY20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:50">
+    <row r="21" spans="1:51">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -3111,14 +3168,17 @@
       <c r="AU21">
         <v>944.9366666666667</v>
       </c>
-      <c r="AW21">
-        <v>18</v>
+      <c r="AW21" t="s">
+        <v>13</v>
       </c>
       <c r="AX21">
+        <v>19</v>
+      </c>
+      <c r="AY21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:50">
+    <row r="22" spans="1:51">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -3239,14 +3299,17 @@
       <c r="AU22">
         <v>945.5433333333334</v>
       </c>
-      <c r="AW22">
-        <v>19</v>
+      <c r="AW22" t="s">
+        <v>13</v>
       </c>
       <c r="AX22">
+        <v>20</v>
+      </c>
+      <c r="AY22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:50">
+    <row r="23" spans="1:51">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -3367,14 +3430,17 @@
       <c r="AU23">
         <v>945.7768333333333</v>
       </c>
-      <c r="AW23">
-        <v>20</v>
+      <c r="AW23" t="s">
+        <v>13</v>
       </c>
       <c r="AX23">
+        <v>21</v>
+      </c>
+      <c r="AY23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:50">
+    <row r="24" spans="1:51">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -3495,14 +3561,17 @@
       <c r="AU24">
         <v>946.3572222222223</v>
       </c>
-      <c r="AW24">
-        <v>21</v>
+      <c r="AW24" t="s">
+        <v>13</v>
       </c>
       <c r="AX24">
+        <v>22</v>
+      </c>
+      <c r="AY24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:50">
+    <row r="25" spans="1:51">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -3623,18 +3692,13 @@
       <c r="AU25">
         <v>915.0172222222222</v>
       </c>
-      <c r="AW25">
-        <v>22</v>
+      <c r="AW25" t="s">
+        <v>13</v>
       </c>
       <c r="AX25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:50">
-      <c r="AW26">
         <v>23</v>
       </c>
-      <c r="AX26">
+      <c r="AY25">
         <v>0</v>
       </c>
     </row>

</xml_diff>